<commit_message>
Added climae to ERD
</commit_message>
<xml_diff>
--- a/ERD/h_a_ERD.xlsx
+++ b/ERD/h_a_ERD.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents1\GitHub\Health_and_Avocados\ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEC152E-A835-46FB-876F-ECCF71E4A0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3521D3-8620-4719-9612-17B41EBFE68F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{A1F7889D-63F4-46FB-A579-0196500EE5CA}"/>
+    <workbookView xWindow="5880" yWindow="3015" windowWidth="20070" windowHeight="16125" firstSheet="1" activeTab="5" xr2:uid="{A1F7889D-63F4-46FB-A579-0196500EE5CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Prices" sheetId="3" r:id="rId2"/>
     <sheet name="Production" sheetId="5" r:id="rId3"/>
-    <sheet name="ERD Diagram" sheetId="4" r:id="rId4"/>
+    <sheet name="Climate" sheetId="6" r:id="rId4"/>
+    <sheet name="ERD Diagram-Source Data" sheetId="4" r:id="rId5"/>
+    <sheet name="ERD Diagram-Consolidation" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="158">
   <si>
     <t>ID</t>
   </si>
@@ -391,6 +393,126 @@
   </si>
   <si>
     <t>AB_2020_AvoProducitonPerWeek</t>
+  </si>
+  <si>
+    <t>ca_climate</t>
+  </si>
+  <si>
+    <t>StateCode</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>YearMonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    PCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   TAVG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   PDSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   PHDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ZNDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   PMDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    CDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    HDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SP01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SP02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SP03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SP06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SP09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SP12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   SP24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   TMIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   TMAX</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>date time</t>
+  </si>
+  <si>
+    <t>CA_State_Climate</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Area within the state - this file is state wide so all 0's</t>
+  </si>
+  <si>
+    <t>year and month</t>
+  </si>
+  <si>
+    <t>percipitation index</t>
+  </si>
+  <si>
+    <t>Temperature index</t>
+  </si>
+  <si>
+    <t>Palmer Drought severity index</t>
+  </si>
+  <si>
+    <t>Palmer Hydrological Drought index</t>
+  </si>
+  <si>
+    <t>Palmer Z-index</t>
+  </si>
+  <si>
+    <t>Modified Palmer Drought Severity index</t>
+  </si>
+  <si>
+    <t>Cooling degree days</t>
+  </si>
+  <si>
+    <t>Heating degree days</t>
+  </si>
+  <si>
+    <t>Standard percipitation index for xx months</t>
+  </si>
+  <si>
+    <t>Temperature max</t>
+  </si>
+  <si>
+    <t>Temperature min</t>
+  </si>
+  <si>
+    <t>2018_2020_Avo_Kaggle_Market_Prices</t>
+  </si>
+  <si>
+    <t>2018_2020_Production</t>
   </si>
 </sst>
 </file>
@@ -551,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -573,6 +695,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,8 +709,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4196,6 +4320,959 @@
         <a:xfrm>
           <a:off x="10591000" y="12465278"/>
           <a:ext cx="760346" cy="785647"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>223546</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>126352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>337847</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>116438</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="Flowchart: Decision 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1383F337-25E8-4B01-9535-4487BD037D0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="835867" y="12683801"/>
+          <a:ext cx="726623" cy="787076"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>337847</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>131115</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>592883</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>145791</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Straight Connector 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AC3F413-2120-4E6E-9194-A8FCA3AB46F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="75" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1562490" y="13077339"/>
+          <a:ext cx="867357" cy="14676"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>340179</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>340179</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>146957</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Straight Connector 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9487B07-0D0A-4B5A-832B-D931D9A13AF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2177143" y="12955944"/>
+          <a:ext cx="0" cy="341345"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>586858</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19440</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>126352</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Straight Connector 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCAF639B-17BC-4540-A881-F62FD18BCDA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:endCxn id="75" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1199179" y="8961276"/>
+          <a:ext cx="44904" cy="3722525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>262424</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>117568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>529662</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>106720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Straight Connector 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B54AD410-1E25-48FF-886B-94601804F2B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="45" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5355383" y="12675017"/>
+          <a:ext cx="549100" cy="377927"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>87475</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>97194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>223546</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>97194</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Straight Connector 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF5B589C-3257-4AD7-B39A-CBD29C08C8BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5462296" y="12849031"/>
+          <a:ext cx="136071" cy="194387"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>262424</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>117568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>529662</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>106720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89CBB412-447F-4E5F-B5E2-0CE42C761D2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5339249" y="12423868"/>
+          <a:ext cx="552988" cy="370152"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>380749</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>108367</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Flowchart: Decision 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0415B235-C488-45F3-97B0-D7BDB06C744D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3905250" y="295275"/>
+          <a:ext cx="742699" cy="784642"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>97046</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03B27AE9-7AFC-4085-B945-2258A133C752}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3648075" y="685800"/>
+          <a:ext cx="257175" cy="1796"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>106571</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2184CCB4-B807-41C2-95F8-0DD9517286C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4667250" y="695325"/>
+          <a:ext cx="257175" cy="1796"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>390274</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>117892</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Flowchart: Decision 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3245B11-2591-4F92-B465-88567E83D58F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591550" y="304800"/>
+          <a:ext cx="742699" cy="784642"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>97046</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{648A684B-FEE6-4EB5-9E56-68BC03555C73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8343900" y="685800"/>
+          <a:ext cx="257175" cy="1796"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB5558B7-7738-47D4-99A6-ABA9CD514D82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9353550" y="704850"/>
+          <a:ext cx="171450" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>56285</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2696785-168A-4DC0-8EC7-A0DAEB32FB7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3800475" y="504825"/>
+          <a:ext cx="0" cy="332510"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>56285</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45B3CEE6-E7D2-4608-84FB-FB26865F8890}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4810125" y="504825"/>
+          <a:ext cx="0" cy="332510"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>75335</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ABF2BCC-99EF-4C25-AB75-B4CD5626C7CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8467725" y="523875"/>
+          <a:ext cx="0" cy="332510"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A85CA89-58A4-4C8A-ACFD-171134B5FADC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9448800" y="904875"/>
+          <a:ext cx="104775" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2B357FA-4614-4E64-9C6C-56BE1C59FB2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9439275" y="895350"/>
+          <a:ext cx="19050" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4536,15 +5613,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -4615,8 +5692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A6CCC-1CD5-40DC-89A7-7AF9B2A6CDD2}">
   <dimension ref="A2:Y76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4645,33 +5722,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="I2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="I2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="21"/>
-      <c r="Q2" s="19" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="23"/>
+      <c r="Q2" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="21"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -4967,7 +6044,7 @@
         <v>86</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="T7" s="5"/>
       <c r="U7">
@@ -5599,15 +6676,15 @@
       <c r="Y18" s="5"/>
     </row>
     <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
       <c r="I19" s="7">
         <v>16</v>
       </c>
@@ -5680,15 +6757,15 @@
       <c r="G21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="21"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -6236,15 +7313,15 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="23"/>
       <c r="I36" s="4">
         <v>14</v>
       </c>
@@ -6386,15 +7463,15 @@
       <c r="G40" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I40" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="21"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="23"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
@@ -6963,15 +8040,15 @@
       </c>
     </row>
     <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I59" s="19" t="s">
+      <c r="I59" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="J59" s="20"/>
-      <c r="K59" s="20"/>
-      <c r="L59" s="20"/>
-      <c r="M59" s="20"/>
-      <c r="N59" s="20"/>
-      <c r="O59" s="21"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="22"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="22"/>
+      <c r="O59" s="23"/>
     </row>
     <row r="60" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I60" s="1" t="s">
@@ -7365,15 +8442,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -7432,7 +8509,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="23">
+      <c r="E5" s="19">
         <v>43107</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -7474,7 +8551,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="24">
+      <c r="E7" s="20">
         <v>45670156</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -7495,7 +8572,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="24">
+      <c r="E8" s="20">
         <v>899349</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -7516,7 +8593,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="24">
+      <c r="E9" s="20">
         <v>519433</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -7537,7 +8614,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="24">
+      <c r="E10" s="20">
         <v>44251374</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -7590,15 +8667,15 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -7657,7 +8734,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="23">
+      <c r="E17" s="19">
         <v>43107</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -7699,7 +8776,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="24">
+      <c r="E19" s="20">
         <v>45670156</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -7720,7 +8797,7 @@
         <v>32</v>
       </c>
       <c r="D20" s="5"/>
-      <c r="E20" s="24">
+      <c r="E20" s="20">
         <v>899349</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -7741,7 +8818,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="E21" s="24">
+      <c r="E21" s="20">
         <v>519433</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -7762,7 +8839,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="24">
+      <c r="E22" s="20">
         <v>44251374</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -7815,15 +8892,15 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -7882,7 +8959,7 @@
         <v>10</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="23">
+      <c r="E29" s="19">
         <v>43107</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -7924,7 +9001,7 @@
         <v>32</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="24">
+      <c r="E31" s="20">
         <v>45670156</v>
       </c>
       <c r="F31" s="5" t="s">
@@ -7945,7 +9022,7 @@
         <v>32</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="24">
+      <c r="E32" s="20">
         <v>899349</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -7966,7 +9043,7 @@
         <v>32</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="24">
+      <c r="E33" s="20">
         <v>519433</v>
       </c>
       <c r="F33" s="5" t="s">
@@ -7987,7 +9064,7 @@
         <v>32</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="24">
+      <c r="E34" s="20">
         <v>44251374</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -8051,11 +9128,495 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76509C0A-71D0-45F7-A862-A6FCFCF84B66}">
+  <dimension ref="A2:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5">
+        <v>201001</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="10">
+        <v>6.48</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="10">
+        <v>45.2</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="10">
+        <v>0.67</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="10">
+        <v>-2.02</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="10">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="10">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="10">
+        <v>491</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="10">
+        <v>0.94</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="10">
+        <v>0.34</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="10">
+        <v>-1.22</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="10">
+        <v>36.6</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>20</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="12">
+        <v>53.7</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF477ADD-6D60-4A52-A419-6123334FD593}">
   <dimension ref="D2:Y97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="44" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="R70" sqref="R70"/>
+    <sheetView topLeftCell="A52" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8127,24 +9688,24 @@
     </row>
     <row r="10" spans="4:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="5"/>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="L10" s="19" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="L10" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="22"/>
-      <c r="V10" s="19" t="s">
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="24"/>
+      <c r="V10" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="24"/>
     </row>
     <row r="11" spans="4:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E11" s="16" t="s">
@@ -8298,7 +9859,7 @@
         <v>86</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="O15" s="6"/>
       <c r="V15" s="4">
@@ -8623,12 +10184,12 @@
       <c r="Y26" s="6"/>
     </row>
     <row r="27" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="24"/>
       <c r="V27" s="7">
         <v>16</v>
       </c>
@@ -8665,12 +10226,12 @@
       <c r="H29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="V29" s="19" t="s">
+      <c r="V29" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="W29" s="20"/>
-      <c r="X29" s="20"/>
-      <c r="Y29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="24"/>
     </row>
     <row r="30" spans="5:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E30" s="4">
@@ -8949,12 +10510,12 @@
       <c r="Y43" s="6"/>
     </row>
     <row r="44" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="24"/>
       <c r="V44" s="4">
         <v>14</v>
       </c>
@@ -9033,12 +10594,12 @@
         <v>31</v>
       </c>
       <c r="H48" s="6"/>
-      <c r="V48" s="19" t="s">
+      <c r="V48" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="W48" s="20"/>
-      <c r="X48" s="20"/>
-      <c r="Y48" s="22"/>
+      <c r="W48" s="22"/>
+      <c r="X48" s="22"/>
+      <c r="Y48" s="24"/>
     </row>
     <row r="49" spans="5:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E49" s="4">
@@ -9323,12 +10884,18 @@
       <c r="Y62" s="6"/>
     </row>
     <row r="63" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L63" s="19" t="s">
+      <c r="E63" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="24"/>
+      <c r="L63" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="M63" s="20"/>
-      <c r="N63" s="20"/>
-      <c r="O63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="24"/>
       <c r="V63" s="4">
         <v>14</v>
       </c>
@@ -9341,6 +10908,18 @@
       <c r="Y63" s="6"/>
     </row>
     <row r="64" spans="5:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="L64" s="1" t="s">
         <v>0</v>
       </c>
@@ -9362,7 +10941,17 @@
       <c r="X64" s="10"/>
       <c r="Y64" s="6"/>
     </row>
-    <row r="65" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E65" s="4">
+        <v>1</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H65" s="6"/>
       <c r="L65" s="4">
         <v>1</v>
       </c>
@@ -9384,7 +10973,17 @@
       <c r="X65" s="12"/>
       <c r="Y65" s="9"/>
     </row>
-    <row r="66" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E66" s="4">
+        <v>2</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H66" s="6"/>
       <c r="L66" s="4">
         <v>2</v>
       </c>
@@ -9396,7 +10995,19 @@
       </c>
       <c r="O66" s="6"/>
     </row>
-    <row r="67" spans="12:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E67" s="4">
+        <v>3</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="L67" s="4">
         <v>3</v>
       </c>
@@ -9407,14 +11018,24 @@
         <v>31</v>
       </c>
       <c r="O67" s="6"/>
-      <c r="V67" s="19" t="s">
+      <c r="V67" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="W67" s="20"/>
-      <c r="X67" s="20"/>
-      <c r="Y67" s="22"/>
-    </row>
-    <row r="68" spans="12:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="W67" s="22"/>
+      <c r="X67" s="22"/>
+      <c r="Y67" s="24"/>
+    </row>
+    <row r="68" spans="5:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="4">
+        <v>4</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H68" s="6"/>
       <c r="L68" s="4">
         <v>4</v>
       </c>
@@ -9438,7 +11059,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E69" s="4">
+        <v>5</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H69" s="6"/>
       <c r="L69" s="4">
         <v>5</v>
       </c>
@@ -9462,7 +11093,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E70" s="4">
+        <v>6</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H70" s="6"/>
       <c r="L70" s="4">
         <v>6</v>
       </c>
@@ -9484,7 +11125,17 @@
       </c>
       <c r="Y70" s="6"/>
     </row>
-    <row r="71" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E71" s="4">
+        <v>7</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H71" s="6"/>
       <c r="L71" s="4">
         <v>7</v>
       </c>
@@ -9506,7 +11157,17 @@
       </c>
       <c r="Y71" s="6"/>
     </row>
-    <row r="72" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E72" s="4">
+        <v>8</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H72" s="6"/>
       <c r="L72" s="4">
         <v>8</v>
       </c>
@@ -9528,7 +11189,17 @@
       </c>
       <c r="Y72" s="6"/>
     </row>
-    <row r="73" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E73" s="4">
+        <v>9</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H73" s="6"/>
       <c r="L73" s="7">
         <v>9</v>
       </c>
@@ -9550,7 +11221,17 @@
       </c>
       <c r="Y73" s="6"/>
     </row>
-    <row r="74" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E74" s="4">
+        <v>10</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H74" s="6"/>
       <c r="V74" s="4">
         <v>6</v>
       </c>
@@ -9562,13 +11243,23 @@
       </c>
       <c r="Y74" s="6"/>
     </row>
-    <row r="75" spans="12:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L75" s="19" t="s">
+    <row r="75" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E75" s="4">
+        <v>11</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" s="6"/>
+      <c r="L75" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="M75" s="20"/>
-      <c r="N75" s="20"/>
-      <c r="O75" s="22"/>
+      <c r="M75" s="22"/>
+      <c r="N75" s="22"/>
+      <c r="O75" s="24"/>
       <c r="V75" s="4">
         <v>7</v>
       </c>
@@ -9580,7 +11271,17 @@
       </c>
       <c r="Y75" s="6"/>
     </row>
-    <row r="76" spans="12:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="4">
+        <v>12</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H76" s="6"/>
       <c r="L76" s="1" t="s">
         <v>0</v>
       </c>
@@ -9604,7 +11305,17 @@
       </c>
       <c r="Y76" s="6"/>
     </row>
-    <row r="77" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E77" s="4">
+        <v>13</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H77" s="6"/>
       <c r="L77" s="4">
         <v>1</v>
       </c>
@@ -9628,7 +11339,17 @@
       </c>
       <c r="Y77" s="6"/>
     </row>
-    <row r="78" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E78" s="4">
+        <v>14</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="6"/>
       <c r="L78" s="4">
         <v>2</v>
       </c>
@@ -9650,7 +11371,17 @@
       </c>
       <c r="Y78" s="6"/>
     </row>
-    <row r="79" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E79" s="4">
+        <v>15</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="6"/>
       <c r="L79" s="4">
         <v>3</v>
       </c>
@@ -9672,7 +11403,17 @@
       </c>
       <c r="Y79" s="6"/>
     </row>
-    <row r="80" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E80" s="4">
+        <v>16</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H80" s="6"/>
       <c r="L80" s="4">
         <v>4</v>
       </c>
@@ -9694,7 +11435,17 @@
       </c>
       <c r="Y80" s="6"/>
     </row>
-    <row r="81" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E81" s="4">
+        <v>17</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H81" s="6"/>
       <c r="L81" s="4">
         <v>5</v>
       </c>
@@ -9716,7 +11467,17 @@
       </c>
       <c r="Y81" s="6"/>
     </row>
-    <row r="82" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E82" s="4">
+        <v>18</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H82" s="6"/>
       <c r="L82" s="4">
         <v>6</v>
       </c>
@@ -9738,7 +11499,17 @@
       </c>
       <c r="Y82" s="6"/>
     </row>
-    <row r="83" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E83" s="4">
+        <v>19</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H83" s="6"/>
       <c r="L83" s="4">
         <v>7</v>
       </c>
@@ -9758,7 +11529,17 @@
       <c r="X83" s="10"/>
       <c r="Y83" s="6"/>
     </row>
-    <row r="84" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E84" s="7">
+        <v>20</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H84" s="9"/>
       <c r="L84" s="4">
         <v>8</v>
       </c>
@@ -9778,7 +11559,7 @@
       <c r="X84" s="12"/>
       <c r="Y84" s="9"/>
     </row>
-    <row r="85" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L85" s="7">
         <v>9</v>
       </c>
@@ -9790,15 +11571,15 @@
       </c>
       <c r="O85" s="9"/>
     </row>
-    <row r="87" spans="12:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L87" s="19" t="s">
+    <row r="87" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L87" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="M87" s="20"/>
-      <c r="N87" s="20"/>
-      <c r="O87" s="22"/>
-    </row>
-    <row r="88" spans="12:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M87" s="22"/>
+      <c r="N87" s="22"/>
+      <c r="O87" s="24"/>
+    </row>
+    <row r="88" spans="5:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L88" s="1" t="s">
         <v>0</v>
       </c>
@@ -9812,7 +11593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L89" s="4">
         <v>1</v>
       </c>
@@ -9826,7 +11607,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L90" s="4">
         <v>2</v>
       </c>
@@ -9838,7 +11619,7 @@
       </c>
       <c r="O90" s="6"/>
     </row>
-    <row r="91" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L91" s="4">
         <v>3</v>
       </c>
@@ -9850,7 +11631,7 @@
       </c>
       <c r="O91" s="6"/>
     </row>
-    <row r="92" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L92" s="4">
         <v>4</v>
       </c>
@@ -9862,7 +11643,7 @@
       </c>
       <c r="O92" s="6"/>
     </row>
-    <row r="93" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L93" s="4">
         <v>5</v>
       </c>
@@ -9874,7 +11655,7 @@
       </c>
       <c r="O93" s="6"/>
     </row>
-    <row r="94" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L94" s="4">
         <v>6</v>
       </c>
@@ -9886,7 +11667,7 @@
       </c>
       <c r="O94" s="6"/>
     </row>
-    <row r="95" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L95" s="4">
         <v>7</v>
       </c>
@@ -9898,7 +11679,7 @@
       </c>
       <c r="O95" s="6"/>
     </row>
-    <row r="96" spans="12:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:25" x14ac:dyDescent="0.25">
       <c r="L96" s="4">
         <v>8</v>
       </c>
@@ -9923,18 +11704,704 @@
       <c r="O97" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="L63:O63"/>
-    <mergeCell ref="L75:O75"/>
-    <mergeCell ref="L87:O87"/>
-    <mergeCell ref="V48:Y48"/>
-    <mergeCell ref="V67:Y67"/>
+  <mergeCells count="12">
+    <mergeCell ref="E63:H63"/>
     <mergeCell ref="L10:O10"/>
     <mergeCell ref="E27:H27"/>
     <mergeCell ref="E44:H44"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="V10:Y10"/>
     <mergeCell ref="V29:Y29"/>
+    <mergeCell ref="L63:O63"/>
+    <mergeCell ref="L75:O75"/>
+    <mergeCell ref="L87:O87"/>
+    <mergeCell ref="V48:Y48"/>
+    <mergeCell ref="V67:Y67"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BB7B71-192D-492B-8FA2-70340F269536}">
+  <dimension ref="C2:R31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="I2" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="24"/>
+      <c r="O2" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="24"/>
+    </row>
+    <row r="3" spans="3:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="O5" s="4">
+        <v>2</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="6"/>
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="O6" s="4">
+        <v>3</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="O7" s="4">
+        <v>4</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="6"/>
+      <c r="I8" s="4">
+        <v>5</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="O8" s="4">
+        <v>5</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="6"/>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C9" s="4">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="6"/>
+      <c r="I9" s="4">
+        <v>6</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="O9" s="4">
+        <v>6</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R9" s="6"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="4">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="6"/>
+      <c r="I10" s="4">
+        <v>7</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="O10" s="4">
+        <v>7</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="6"/>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="4">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="6"/>
+      <c r="I11" s="4">
+        <v>8</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="O11" s="4">
+        <v>8</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="6"/>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="4">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="6"/>
+      <c r="I12" s="7">
+        <v>9</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="O12" s="4">
+        <v>9</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="6"/>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="4">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="6"/>
+      <c r="O13" s="4">
+        <v>10</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" s="6"/>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="4">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="6"/>
+      <c r="O14" s="4">
+        <v>11</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="6"/>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C15" s="4">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="6"/>
+      <c r="O15" s="4">
+        <v>12</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R15" s="6"/>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="6"/>
+      <c r="O16" s="4">
+        <v>13</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16" s="6"/>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C17" s="4">
+        <v>14</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="6"/>
+      <c r="O17" s="4">
+        <v>14</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R17" s="6"/>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="25">
+        <v>15</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="O18" s="4">
+        <v>15</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18" s="6"/>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19" s="25">
+        <v>16</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="O19" s="4">
+        <v>16</v>
+      </c>
+      <c r="P19" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R19" s="6"/>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="25">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="O20" s="4">
+        <v>17</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C21" s="25">
+        <v>18</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="O21" s="4">
+        <v>18</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R21" s="6"/>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C22" s="25">
+        <v>19</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="O22" s="4">
+        <v>19</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R22" s="6"/>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C23" s="25">
+        <v>20</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="O23" s="7">
+        <v>20</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R23" s="9"/>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C24" s="25">
+        <v>21</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C25" s="25">
+        <v>22</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C26" s="25">
+        <v>23</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C27" s="25">
+        <v>24</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C28" s="25">
+        <v>25</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="25">
+        <v>26</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="25">
+        <v>27</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="26">
+        <v>28</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="O2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>